<commit_message>
updates to joss submission
</commit_message>
<xml_diff>
--- a/Travis_County/Documentation/Travis_County_2017_bg_SVI.xlsx
+++ b/Travis_County/Documentation/Travis_County_2017_bg_SVI.xlsx
@@ -462,7 +462,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>['PPUNIT' 'QEXTRCT' 'QEDLESHI' 'QSERV' 'QHISPC' 'QESL' 'QNOHLTH' 'QFHH'
+          <t>['QEXTRCT' 'QEDLESHI' 'QESL' 'QNOHLTH' 'PPUNIT' 'QSERV' 'QHISPC' 'QFHH'
  'PERCAP']</t>
         </is>
       </c>
@@ -497,7 +497,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>['MEDAGE' 'QAGEDEP' 'QSSBEN']</t>
+          <t>['MEDAGE' 'QSSBEN' 'QAGEDEP']</t>
         </is>
       </c>
     </row>
@@ -531,7 +531,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>['PPUNIT' 'QRENTER' 'QPOVTY' 'QNOAUTO']</t>
+          <t>['PPUNIT' 'QRENTER' 'QNOAUTO' 'QPOVTY']</t>
         </is>
       </c>
     </row>
@@ -584,155 +584,155 @@
     <row r="2">
       <c r="A2" s="1" t="inlineStr">
         <is>
-          <t>PPUNIT</t>
+          <t>QEXTRCT</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>0.7302277635614846</v>
+        <v>0.7677512013307708</v>
       </c>
       <c r="C2" t="n">
-        <v>-0.004620265553080765</v>
+        <v>0.1449653481766418</v>
       </c>
       <c r="D2" t="n">
-        <v>-0.1512975031741777</v>
+        <v>0.01129679077873671</v>
       </c>
       <c r="E2" t="n">
-        <v>0.0545872990130594</v>
+        <v>-0.2382017695991725</v>
       </c>
       <c r="F2" t="n">
-        <v>-0.4752714233751672</v>
+        <v>0.09278788174314587</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="1" t="inlineStr">
         <is>
-          <t>QEXTRCT</t>
+          <t>QEDLESHI</t>
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.7677511913183374</v>
+        <v>0.8777939278338194</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1449653505664406</v>
+        <v>0.213077928978771</v>
       </c>
       <c r="D3" t="n">
-        <v>0.01129678599078328</v>
+        <v>-0.01839361500093432</v>
       </c>
       <c r="E3" t="n">
-        <v>-0.2382017650496178</v>
+        <v>-0.1076883429731288</v>
       </c>
       <c r="F3" t="n">
-        <v>0.09278788561119072</v>
+        <v>0.1846338367566293</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="1" t="inlineStr">
         <is>
-          <t>QEDLESHI</t>
+          <t>QESL</t>
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.877793933021792</v>
+        <v>0.8009661475849839</v>
       </c>
       <c r="C4" t="n">
-        <v>0.2130779235964615</v>
+        <v>0.1517950795169672</v>
       </c>
       <c r="D4" t="n">
-        <v>-0.01839360962230008</v>
+        <v>-0.03424774416423925</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.1076883442393492</v>
+        <v>-0.2374898287916476</v>
       </c>
       <c r="F4" t="n">
-        <v>0.1846338473713447</v>
+        <v>0.2037776713559489</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="1" t="inlineStr">
         <is>
-          <t>QSERV</t>
+          <t>QNOHLTH</t>
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.5817049372257884</v>
+        <v>0.6889886573070284</v>
       </c>
       <c r="C5" t="n">
-        <v>0.3577287406387448</v>
+        <v>0.414959225541808</v>
       </c>
       <c r="D5" t="n">
-        <v>-0.2244058824899562</v>
+        <v>-0.1190897065630508</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.03201466777107302</v>
+        <v>-0.1154839642310589</v>
       </c>
       <c r="F5" t="n">
-        <v>0.2754259478725354</v>
+        <v>0.2786568866560452</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="1" t="inlineStr">
         <is>
-          <t>QHISPC</t>
+          <t>PPUNIT</t>
         </is>
       </c>
       <c r="B6" t="n">
-        <v>0.8328587050403832</v>
+        <v>0.7302277711183555</v>
       </c>
       <c r="C6" t="n">
-        <v>0.3339037450738082</v>
+        <v>-0.004620272024895255</v>
       </c>
       <c r="D6" t="n">
-        <v>-0.1364957904807652</v>
+        <v>-0.1512975164200612</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.1269704308693348</v>
+        <v>0.05458730556150756</v>
       </c>
       <c r="F6" t="n">
-        <v>0.09670565249334595</v>
+        <v>-0.4752714593490717</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="1" t="inlineStr">
         <is>
-          <t>QESL</t>
+          <t>QSERV</t>
         </is>
       </c>
       <c r="B7" t="n">
-        <v>0.8009661449175541</v>
+        <v>0.581704943683128</v>
       </c>
       <c r="C7" t="n">
-        <v>0.1517950777004842</v>
+        <v>0.3577287418172193</v>
       </c>
       <c r="D7" t="n">
-        <v>-0.03424774394570817</v>
+        <v>-0.2244058884840431</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.2374898280304555</v>
+        <v>-0.03201466441996235</v>
       </c>
       <c r="F7" t="n">
-        <v>0.2037776768212274</v>
+        <v>0.2754259447697267</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="1" t="inlineStr">
         <is>
-          <t>QNOHLTH</t>
+          <t>QHISPC</t>
         </is>
       </c>
       <c r="B8" t="n">
-        <v>0.6889886581195417</v>
+        <v>0.8328587063035261</v>
       </c>
       <c r="C8" t="n">
-        <v>0.4149592262288362</v>
+        <v>0.3339037468887154</v>
       </c>
       <c r="D8" t="n">
-        <v>-0.1190896999544257</v>
+        <v>-0.1364957918037546</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.115483966344917</v>
+        <v>-0.126970430831828</v>
       </c>
       <c r="F8" t="n">
-        <v>0.278656896370206</v>
+        <v>0.09670564462395792</v>
       </c>
     </row>
     <row r="9">
@@ -742,19 +742,19 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>0.5630560174848608</v>
+        <v>0.5630560183163126</v>
       </c>
       <c r="C9" t="n">
-        <v>0.3008187145654854</v>
+        <v>0.3008187155964411</v>
       </c>
       <c r="D9" t="n">
-        <v>-0.095513173626251</v>
+        <v>-0.09551317755867508</v>
       </c>
       <c r="E9" t="n">
-        <v>0.2634165315403454</v>
+        <v>0.2634165381813704</v>
       </c>
       <c r="F9" t="n">
-        <v>-0.03178269348764106</v>
+        <v>-0.03178270184700521</v>
       </c>
     </row>
     <row r="10">
@@ -764,19 +764,19 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>0.4895374246541067</v>
+        <v>0.4895374235147206</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7214540924412403</v>
+        <v>0.7214540992653554</v>
       </c>
       <c r="D10" t="n">
-        <v>-0.2685725759671641</v>
+        <v>-0.2685725828240927</v>
       </c>
       <c r="E10" t="n">
-        <v>0.05482089860683299</v>
+        <v>0.05482090093234365</v>
       </c>
       <c r="F10" t="n">
-        <v>0.18312535117927</v>
+        <v>0.1831253412505047</v>
       </c>
     </row>
     <row r="11">
@@ -786,19 +786,19 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>0.2150971440109055</v>
+        <v>0.2150971482753866</v>
       </c>
       <c r="C11" t="n">
-        <v>0.8701305572213086</v>
+        <v>0.870130548924468</v>
       </c>
       <c r="D11" t="n">
-        <v>-0.1729034313348966</v>
+        <v>-0.1729034375056023</v>
       </c>
       <c r="E11" t="n">
-        <v>-0.0142515365962387</v>
+        <v>-0.0142515353605643</v>
       </c>
       <c r="F11" t="n">
-        <v>0.2948729874682595</v>
+        <v>0.2948729845659209</v>
       </c>
     </row>
     <row r="12">
@@ -808,19 +808,19 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>0.3857664778128806</v>
+        <v>0.3857664718237477</v>
       </c>
       <c r="C12" t="n">
-        <v>0.8013369872884633</v>
+        <v>0.8013370028956395</v>
       </c>
       <c r="D12" t="n">
-        <v>-0.03601197710565474</v>
+        <v>-0.03601197413356935</v>
       </c>
       <c r="E12" t="n">
-        <v>-0.02873185494301043</v>
+        <v>-0.02873185735955726</v>
       </c>
       <c r="F12" t="n">
-        <v>-0.03016150205507568</v>
+        <v>-0.03016150937756498</v>
       </c>
     </row>
     <row r="13">
@@ -830,63 +830,63 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>-0.310547262470854</v>
+        <v>-0.3105472617371984</v>
       </c>
       <c r="C13" t="n">
-        <v>-0.246538429426827</v>
+        <v>-0.2465384280778078</v>
       </c>
       <c r="D13" t="n">
-        <v>0.7910361807365249</v>
+        <v>0.7910361908750342</v>
       </c>
       <c r="E13" t="n">
-        <v>-0.01289474326237975</v>
+        <v>-0.01289474291113122</v>
       </c>
       <c r="F13" t="n">
-        <v>-0.2717085841605006</v>
+        <v>-0.2717085724916322</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="1" t="inlineStr">
         <is>
-          <t>QAGEDEP</t>
+          <t>QSSBEN</t>
         </is>
       </c>
       <c r="B14" t="n">
-        <v>-0.04282432259531188</v>
+        <v>0.01836498286088173</v>
       </c>
       <c r="C14" t="n">
-        <v>-0.1184872960388995</v>
+        <v>-0.05367045675897775</v>
       </c>
       <c r="D14" t="n">
-        <v>0.6543380977114776</v>
+        <v>0.7773306962764825</v>
       </c>
       <c r="E14" t="n">
-        <v>0.6427560425405702</v>
+        <v>0.136209976584241</v>
       </c>
       <c r="F14" t="n">
-        <v>-0.1139548231976987</v>
+        <v>-0.1455945068606067</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="1" t="inlineStr">
         <is>
-          <t>QSSBEN</t>
+          <t>QAGEDEP</t>
         </is>
       </c>
       <c r="B15" t="n">
-        <v>0.01836498062193265</v>
+        <v>-0.04282432190847357</v>
       </c>
       <c r="C15" t="n">
-        <v>-0.0536704550579051</v>
+        <v>-0.1184872960740083</v>
       </c>
       <c r="D15" t="n">
-        <v>0.7773307026735096</v>
+        <v>0.6543380961981018</v>
       </c>
       <c r="E15" t="n">
-        <v>0.1362099709473573</v>
+        <v>0.6427560452936805</v>
       </c>
       <c r="F15" t="n">
-        <v>-0.1455945104196087</v>
+        <v>-0.1139548183463203</v>
       </c>
     </row>
     <row r="16">
@@ -896,19 +896,19 @@
         </is>
       </c>
       <c r="B16" t="n">
-        <v>-0.2416846120371116</v>
+        <v>-0.2416846133880868</v>
       </c>
       <c r="C16" t="n">
-        <v>0.08178103396692342</v>
+        <v>0.08178103263001013</v>
       </c>
       <c r="D16" t="n">
-        <v>-0.02959552843600554</v>
+        <v>-0.02959553031661272</v>
       </c>
       <c r="E16" t="n">
-        <v>0.7849928975866307</v>
+        <v>0.7849929020395576</v>
       </c>
       <c r="F16" t="n">
-        <v>0.003645846115950876</v>
+        <v>0.003645848475871107</v>
       </c>
     </row>
     <row r="17">
@@ -918,19 +918,19 @@
         </is>
       </c>
       <c r="B17" t="n">
-        <v>-0.04556235852184229</v>
+        <v>-0.04556236170050956</v>
       </c>
       <c r="C17" t="n">
-        <v>-0.05659266818184682</v>
+        <v>-0.05659266582526922</v>
       </c>
       <c r="D17" t="n">
-        <v>0.1671554317435279</v>
+        <v>0.1671554332667903</v>
       </c>
       <c r="E17" t="n">
-        <v>0.8778432103517438</v>
+        <v>0.8778431990123544</v>
       </c>
       <c r="F17" t="n">
-        <v>-0.0242050155512474</v>
+        <v>-0.0242050142911791</v>
       </c>
     </row>
     <row r="18">
@@ -940,63 +940,63 @@
         </is>
       </c>
       <c r="B18" t="n">
-        <v>0.01759023452870938</v>
+        <v>0.01759024404216022</v>
       </c>
       <c r="C18" t="n">
-        <v>0.2288188117534955</v>
+        <v>0.2288188101098284</v>
       </c>
       <c r="D18" t="n">
-        <v>-0.4234144287363591</v>
+        <v>-0.4234144374084097</v>
       </c>
       <c r="E18" t="n">
-        <v>-0.09662324417498865</v>
+        <v>-0.09662324389171931</v>
       </c>
       <c r="F18" t="n">
-        <v>0.7659446311347016</v>
+        <v>0.7659446219419647</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="1" t="inlineStr">
         <is>
-          <t>QPOVTY</t>
+          <t>QNOAUTO</t>
         </is>
       </c>
       <c r="B19" t="n">
-        <v>0.3701334402679973</v>
+        <v>0.1660837693831291</v>
       </c>
       <c r="C19" t="n">
-        <v>0.157633475615365</v>
+        <v>0.06295541374020226</v>
       </c>
       <c r="D19" t="n">
-        <v>-0.3817953714200449</v>
+        <v>-0.1064187480161447</v>
       </c>
       <c r="E19" t="n">
-        <v>0.08010853061944063</v>
+        <v>-0.01530325772402283</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4611334680510979</v>
+        <v>0.6312035357109876</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="1" t="inlineStr">
         <is>
-          <t>QNOAUTO</t>
+          <t>QPOVTY</t>
         </is>
       </c>
       <c r="B20" t="n">
-        <v>0.1660837593915019</v>
+        <v>0.3701334443131513</v>
       </c>
       <c r="C20" t="n">
-        <v>0.06295541833532646</v>
+        <v>0.157633475077385</v>
       </c>
       <c r="D20" t="n">
-        <v>-0.1064187384595324</v>
+        <v>-0.3817953811110359</v>
       </c>
       <c r="E20" t="n">
-        <v>-0.01530326265014326</v>
+        <v>0.08010853240336936</v>
       </c>
       <c r="F20" t="n">
-        <v>0.6312035354106397</v>
+        <v>0.4611334541988245</v>
       </c>
     </row>
   </sheetData>
@@ -1133,34 +1133,34 @@
         <v>1.01176302747226</v>
       </c>
       <c r="I2" t="n">
-        <v>4.839746450906217</v>
+        <v>4.839746425340321</v>
       </c>
       <c r="J2" t="n">
-        <v>3.422021206471405</v>
+        <v>3.422021238437344</v>
       </c>
       <c r="K2" t="n">
-        <v>2.232417349047039</v>
+        <v>2.232417334146756</v>
       </c>
       <c r="L2" t="n">
-        <v>2.056337888802102</v>
+        <v>2.056337886114042</v>
       </c>
       <c r="M2" t="n">
-        <v>2.044708468765052</v>
+        <v>2.044708471301834</v>
       </c>
       <c r="N2" t="n">
-        <v>5.117234758546898</v>
+        <v>5.117234792812528</v>
       </c>
       <c r="O2" t="n">
-        <v>2.680150597288756</v>
+        <v>2.680150619567169</v>
       </c>
       <c r="P2" t="n">
-        <v>2.243476568521099</v>
+        <v>2.243476605342225</v>
       </c>
       <c r="Q2" t="n">
-        <v>2.066288183410713</v>
+        <v>2.066288181755519</v>
       </c>
       <c r="R2" t="n">
-        <v>1.901714796742297</v>
+        <v>1.901714776046654</v>
       </c>
     </row>
     <row r="3">
@@ -1191,34 +1191,34 @@
         <v>0.03747270472119483</v>
       </c>
       <c r="I3" t="n">
-        <v>0.2304641167098199</v>
+        <v>0.2304641154923962</v>
       </c>
       <c r="J3" t="n">
-        <v>0.1629533907843526</v>
+        <v>0.1629533923065402</v>
       </c>
       <c r="K3" t="n">
-        <v>0.106305588049859</v>
+        <v>0.1063055873403217</v>
       </c>
       <c r="L3" t="n">
-        <v>0.09792085184771913</v>
+        <v>0.09792085171971628</v>
       </c>
       <c r="M3" t="n">
-        <v>0.09736706994119293</v>
+        <v>0.09736707006199209</v>
       </c>
       <c r="N3" t="n">
-        <v>0.2693281451866789</v>
+        <v>0.2693281469901331</v>
       </c>
       <c r="O3" t="n">
-        <v>0.1410605577520398</v>
+        <v>0.1410605589245879</v>
       </c>
       <c r="P3" t="n">
-        <v>0.1180777141326894</v>
+        <v>0.1180777160706434</v>
       </c>
       <c r="Q3" t="n">
-        <v>0.1087520096531954</v>
+        <v>0.10875200956608</v>
       </c>
       <c r="R3" t="n">
-        <v>0.1000902524601209</v>
+        <v>0.1000902513708765</v>
       </c>
     </row>
     <row r="4">
@@ -1249,34 +1249,34 @@
         <v>0.6381373038352784</v>
       </c>
       <c r="I4" t="n">
-        <v>0.2304641167098199</v>
+        <v>0.2304641154923962</v>
       </c>
       <c r="J4" t="n">
-        <v>0.3934175074941725</v>
+        <v>0.3934175077989364</v>
       </c>
       <c r="K4" t="n">
-        <v>0.4997230955440315</v>
+        <v>0.4997230951392581</v>
       </c>
       <c r="L4" t="n">
-        <v>0.5976439473917506</v>
+        <v>0.5976439468589744</v>
       </c>
       <c r="M4" t="n">
-        <v>0.6950110173329436</v>
+        <v>0.6950110169209665</v>
       </c>
       <c r="N4" t="n">
-        <v>0.2693281451866789</v>
+        <v>0.2693281469901331</v>
       </c>
       <c r="O4" t="n">
-        <v>0.4103887029387187</v>
+        <v>0.4103887059147209</v>
       </c>
       <c r="P4" t="n">
-        <v>0.5284664170714081</v>
+        <v>0.5284664219853643</v>
       </c>
       <c r="Q4" t="n">
-        <v>0.6372184267246035</v>
+        <v>0.6372184315514443</v>
       </c>
       <c r="R4" t="n">
-        <v>0.7373086791847243</v>
+        <v>0.7373086829223208</v>
       </c>
     </row>
     <row r="5">
@@ -1307,34 +1307,34 @@
         <v>0.05872200934811297</v>
       </c>
       <c r="I5" t="n">
-        <v>0.3315977890454311</v>
+        <v>0.3315977874903292</v>
       </c>
       <c r="J5" t="n">
-        <v>0.2344615937308087</v>
+        <v>0.2344615960599521</v>
       </c>
       <c r="K5" t="n">
-        <v>0.1529552559580988</v>
+        <v>0.1529552550278643</v>
       </c>
       <c r="L5" t="n">
-        <v>0.1408910785666155</v>
+        <v>0.1408910784659567</v>
       </c>
       <c r="M5" t="n">
-        <v>0.140094282699046</v>
+        <v>0.1400942829558977</v>
       </c>
       <c r="N5" t="n">
-        <v>0.3652854669830921</v>
+        <v>0.3652854675773677</v>
       </c>
       <c r="O5" t="n">
-        <v>0.1913181842752981</v>
+        <v>0.1913181848957682</v>
       </c>
       <c r="P5" t="n">
-        <v>0.1601469200976358</v>
+        <v>0.1601469219142283</v>
       </c>
       <c r="Q5" t="n">
-        <v>0.1474986158761178</v>
+        <v>0.1474986150102582</v>
       </c>
       <c r="R5" t="n">
-        <v>0.1357508127678562</v>
+        <v>0.1357508106023777</v>
       </c>
     </row>
   </sheetData>
@@ -1390,19 +1390,19 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>5.117234758546898</v>
+        <v>5.117234792812528</v>
       </c>
       <c r="C2" t="n">
-        <v>2.680150597288756</v>
+        <v>2.680150619567169</v>
       </c>
       <c r="D2" t="n">
-        <v>2.243476568521099</v>
+        <v>2.243476605342225</v>
       </c>
       <c r="E2" t="n">
-        <v>2.066288183410713</v>
+        <v>2.066288181755519</v>
       </c>
       <c r="F2" t="n">
-        <v>1.901714796742297</v>
+        <v>1.901714776046654</v>
       </c>
     </row>
     <row r="3">
@@ -1412,19 +1412,19 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>0.2693281451866789</v>
+        <v>0.2693281469901331</v>
       </c>
       <c r="C3" t="n">
-        <v>0.1410605577520398</v>
+        <v>0.1410605589245879</v>
       </c>
       <c r="D3" t="n">
-        <v>0.1180777141326894</v>
+        <v>0.1180777160706434</v>
       </c>
       <c r="E3" t="n">
-        <v>0.1087520096531954</v>
+        <v>0.10875200956608</v>
       </c>
       <c r="F3" t="n">
-        <v>0.1000902524601209</v>
+        <v>0.1000902513708765</v>
       </c>
     </row>
     <row r="4">
@@ -1434,19 +1434,19 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>0.2693281451866789</v>
+        <v>0.2693281469901331</v>
       </c>
       <c r="C4" t="n">
-        <v>0.4103887029387187</v>
+        <v>0.4103887059147209</v>
       </c>
       <c r="D4" t="n">
-        <v>0.5284664170714081</v>
+        <v>0.5284664219853643</v>
       </c>
       <c r="E4" t="n">
-        <v>0.6372184267246035</v>
+        <v>0.6372184315514443</v>
       </c>
       <c r="F4" t="n">
-        <v>0.7373086791847243</v>
+        <v>0.7373086829223208</v>
       </c>
     </row>
     <row r="5">
@@ -1456,19 +1456,19 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>0.3652854669830921</v>
+        <v>0.3652854675773677</v>
       </c>
       <c r="C5" t="n">
-        <v>0.1913181842752981</v>
+        <v>0.1913181848957682</v>
       </c>
       <c r="D5" t="n">
-        <v>0.1601469200976358</v>
+        <v>0.1601469219142283</v>
       </c>
       <c r="E5" t="n">
-        <v>0.1474986158761178</v>
+        <v>0.1474986150102582</v>
       </c>
       <c r="F5" t="n">
-        <v>0.1357508127678562</v>
+        <v>0.1357508106023777</v>
       </c>
     </row>
   </sheetData>
@@ -1508,7 +1508,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>[['PPUNIT', 'QEXTRCT', 'QEDLESHI', 'QSERV', 'QHISPC', 'QESL', 'QNOHLTH', 'QFHH', 'PERCAP', 'QRICH', 'MDHSEVAL', 'MEDAGE', 'QAGEDEP', 'QSSBEN', 'QFEMLBR', 'QFEMALE', 'QRENTER', 'QPOVTY', 'QNOAUTO']]</t>
+          <t>[['QEXTRCT', 'QEDLESHI', 'QESL', 'QNOHLTH', 'PPUNIT', 'QSERV', 'QHISPC', 'QFHH', 'PERCAP', 'QRICH', 'MDHSEVAL', 'MEDAGE', 'QSSBEN', 'QAGEDEP', 'QFEMLBR', 'QFEMALE', 'QRENTER', 'QNOAUTO', 'QPOVTY']]</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">

</xml_diff>